<commit_message>
opt@3.1.1# update release backlog
</commit_message>
<xml_diff>
--- a/VersionRecords/Version3.1.1/版本Bug和特性计划及评审表v3.1.1_ALL.xlsx
+++ b/VersionRecords/Version3.1.1/版本Bug和特性计划及评审表v3.1.1_ALL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\worktools\GitRepository_bak\Mogo_Doc\VersionRecords\Version3.1.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\mogo_git\Mogo_Doc\VersionRecords\Version3.1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'版本3.1.1新特性|Fix Bug'!$A$1:$T$1</definedName>
   </definedNames>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="285">
   <si>
     <t>No</t>
   </si>
@@ -1100,6 +1100,34 @@
   </si>
   <si>
     <t>房源推荐排序规则实时更新</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>【BS】职业房东录入，必填信息提交错误后，无法再次提交问题</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>蒋文</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>费用类型设置只有双击才能勾选</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>蒋文</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>发现组</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1394,7 +1422,7 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1514,6 +1542,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -1877,10 +1908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T98"/>
+  <dimension ref="A1:T100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4209,42 +4240,40 @@
         <v>55</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>170</v>
+        <v>278</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>171</v>
+        <v>279</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>172</v>
+        <v>32</v>
       </c>
       <c r="F56" s="21">
         <v>42478</v>
       </c>
       <c r="G56" s="21" t="s">
-        <v>172</v>
+        <v>32</v>
       </c>
       <c r="H56" s="21">
         <v>42478</v>
       </c>
       <c r="I56" s="8"/>
       <c r="J56" s="20" t="s">
-        <v>174</v>
+        <v>280</v>
       </c>
       <c r="K56" s="8" t="s">
-        <v>176</v>
+        <v>124</v>
       </c>
       <c r="L56" s="8"/>
       <c r="M56" s="20"/>
       <c r="N56" s="21"/>
       <c r="O56" s="20"/>
-      <c r="P56" s="25"/>
-      <c r="Q56" s="25"/>
-      <c r="R56" s="25" t="s">
-        <v>177</v>
-      </c>
+      <c r="P56" s="17"/>
+      <c r="Q56" s="17"/>
+      <c r="R56" s="17"/>
       <c r="S56" s="26"/>
       <c r="T56" s="27"/>
     </row>
@@ -4252,14 +4281,14 @@
       <c r="A57" s="8">
         <v>56</v>
       </c>
-      <c r="B57" s="24" t="s">
-        <v>178</v>
+      <c r="B57" s="40" t="s">
+        <v>281</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>179</v>
+        <v>150</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>32</v>
@@ -4268,25 +4297,25 @@
         <v>42478</v>
       </c>
       <c r="G57" s="21" t="s">
-        <v>172</v>
+        <v>282</v>
       </c>
       <c r="H57" s="21">
         <v>42478</v>
       </c>
       <c r="I57" s="8"/>
       <c r="J57" s="20" t="s">
-        <v>180</v>
+        <v>283</v>
       </c>
       <c r="K57" s="8" t="s">
-        <v>181</v>
+        <v>284</v>
       </c>
       <c r="L57" s="8"/>
       <c r="M57" s="20"/>
       <c r="N57" s="21"/>
       <c r="O57" s="20"/>
-      <c r="P57" s="25"/>
-      <c r="Q57" s="25"/>
-      <c r="R57" s="25"/>
+      <c r="P57" s="17"/>
+      <c r="Q57" s="17"/>
+      <c r="R57" s="17"/>
       <c r="S57" s="26"/>
       <c r="T57" s="27"/>
     </row>
@@ -4295,29 +4324,29 @@
         <v>57</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>139</v>
+        <v>28</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>32</v>
+        <v>172</v>
       </c>
       <c r="F58" s="21">
         <v>42478</v>
       </c>
       <c r="G58" s="21" t="s">
-        <v>32</v>
+        <v>172</v>
       </c>
       <c r="H58" s="21">
         <v>42478</v>
       </c>
       <c r="I58" s="8"/>
       <c r="J58" s="20" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="K58" s="8" t="s">
         <v>176</v>
@@ -4328,7 +4357,9 @@
       <c r="O58" s="20"/>
       <c r="P58" s="25"/>
       <c r="Q58" s="25"/>
-      <c r="R58" s="25"/>
+      <c r="R58" s="25" t="s">
+        <v>177</v>
+      </c>
       <c r="S58" s="26"/>
       <c r="T58" s="27"/>
     </row>
@@ -4337,29 +4368,29 @@
         <v>58</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>139</v>
+        <v>28</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>186</v>
+        <v>32</v>
       </c>
       <c r="F59" s="21">
         <v>42478</v>
       </c>
       <c r="G59" s="21" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="H59" s="21">
         <v>42478</v>
       </c>
       <c r="I59" s="8"/>
       <c r="J59" s="20" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="K59" s="8" t="s">
         <v>181</v>
@@ -4379,22 +4410,22 @@
         <v>59</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>139</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>190</v>
+        <v>32</v>
       </c>
       <c r="F60" s="21">
         <v>42478</v>
       </c>
       <c r="G60" s="21" t="s">
-        <v>130</v>
+        <v>32</v>
       </c>
       <c r="H60" s="21">
         <v>42478</v>
@@ -4404,7 +4435,7 @@
         <v>173</v>
       </c>
       <c r="K60" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="L60" s="8"/>
       <c r="M60" s="20"/>
@@ -4421,13 +4452,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="24" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>28</v>
+        <v>139</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>186</v>
@@ -4436,17 +4467,17 @@
         <v>42478</v>
       </c>
       <c r="G61" s="21" t="s">
-        <v>32</v>
+        <v>186</v>
       </c>
       <c r="H61" s="21">
         <v>42478</v>
       </c>
       <c r="I61" s="8"/>
       <c r="J61" s="20" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="K61" s="8" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="L61" s="8"/>
       <c r="M61" s="20"/>
@@ -4463,13 +4494,13 @@
         <v>61</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>139</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>190</v>
@@ -4485,10 +4516,10 @@
       </c>
       <c r="I62" s="8"/>
       <c r="J62" s="20" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="K62" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L62" s="8"/>
       <c r="M62" s="20"/>
@@ -4505,32 +4536,32 @@
         <v>62</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>196</v>
+        <v>28</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>130</v>
+        <v>186</v>
       </c>
       <c r="F63" s="21">
         <v>42478</v>
       </c>
       <c r="G63" s="21" t="s">
-        <v>130</v>
+        <v>32</v>
       </c>
       <c r="H63" s="21">
         <v>42478</v>
       </c>
       <c r="I63" s="8"/>
       <c r="J63" s="20" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="K63" s="8" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="L63" s="8"/>
       <c r="M63" s="20"/>
@@ -4547,16 +4578,16 @@
         <v>63</v>
       </c>
       <c r="B64" s="24" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>139</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="F64" s="21">
         <v>42478</v>
@@ -4569,10 +4600,10 @@
       </c>
       <c r="I64" s="8"/>
       <c r="J64" s="20" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="K64" s="8" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="L64" s="8"/>
       <c r="M64" s="20"/>
@@ -4589,22 +4620,22 @@
         <v>64</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>139</v>
+        <v>196</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>190</v>
+        <v>130</v>
       </c>
       <c r="F65" s="21">
         <v>42478</v>
       </c>
       <c r="G65" s="21" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="H65" s="21">
         <v>42478</v>
@@ -4614,7 +4645,7 @@
         <v>199</v>
       </c>
       <c r="K65" s="8" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="L65" s="8"/>
       <c r="M65" s="20"/>
@@ -4631,13 +4662,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="24" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>186</v>
@@ -4646,14 +4677,14 @@
         <v>42478</v>
       </c>
       <c r="G66" s="21" t="s">
-        <v>190</v>
+        <v>130</v>
       </c>
       <c r="H66" s="21">
         <v>42478</v>
       </c>
       <c r="I66" s="8"/>
       <c r="J66" s="20" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="K66" s="8" t="s">
         <v>181</v>
@@ -4673,32 +4704,32 @@
         <v>66</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>130</v>
+        <v>190</v>
       </c>
       <c r="F67" s="21">
         <v>42478</v>
       </c>
       <c r="G67" s="21" t="s">
-        <v>130</v>
+        <v>32</v>
       </c>
       <c r="H67" s="21">
         <v>42478</v>
       </c>
       <c r="I67" s="8"/>
       <c r="J67" s="20" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="K67" s="8" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="L67" s="8"/>
       <c r="M67" s="20"/>
@@ -4715,29 +4746,29 @@
         <v>67</v>
       </c>
       <c r="B68" s="24" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>130</v>
+        <v>186</v>
       </c>
       <c r="F68" s="21">
         <v>42478</v>
       </c>
       <c r="G68" s="21" t="s">
-        <v>130</v>
+        <v>190</v>
       </c>
       <c r="H68" s="21">
         <v>42478</v>
       </c>
       <c r="I68" s="8"/>
       <c r="J68" s="20" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="K68" s="8" t="s">
         <v>181</v>
@@ -4757,32 +4788,32 @@
         <v>68</v>
       </c>
       <c r="B69" s="24" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="F69" s="21">
         <v>42478</v>
       </c>
       <c r="G69" s="21" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="H69" s="21">
         <v>42478</v>
       </c>
       <c r="I69" s="8"/>
       <c r="J69" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K69" s="8" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="L69" s="8"/>
       <c r="M69" s="20"/>
@@ -4794,104 +4825,102 @@
       <c r="S69" s="26"/>
       <c r="T69" s="27"/>
     </row>
-    <row r="70" spans="1:20" s="37" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:20" s="28" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A70" s="8">
         <v>69</v>
       </c>
-      <c r="B70" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="C70" s="31" t="s">
-        <v>211</v>
-      </c>
-      <c r="D70" s="31" t="s">
-        <v>212</v>
-      </c>
-      <c r="E70" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="F70" s="32">
-        <v>42475</v>
-      </c>
-      <c r="G70" s="32" t="s">
-        <v>213</v>
-      </c>
-      <c r="H70" s="32">
-        <v>42475</v>
-      </c>
-      <c r="I70" s="31"/>
-      <c r="J70" s="33" t="s">
-        <v>214</v>
-      </c>
-      <c r="K70" s="31" t="s">
-        <v>215</v>
-      </c>
-      <c r="L70" s="31"/>
-      <c r="M70" s="33"/>
-      <c r="N70" s="32"/>
-      <c r="O70" s="33"/>
-      <c r="P70" s="34"/>
-      <c r="Q70" s="34"/>
-      <c r="R70" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="S70" s="35"/>
-      <c r="T70" s="36"/>
-    </row>
-    <row r="71" spans="1:20" s="37" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B70" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="E70" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="F70" s="21">
+        <v>42478</v>
+      </c>
+      <c r="G70" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="H70" s="21">
+        <v>42478</v>
+      </c>
+      <c r="I70" s="8"/>
+      <c r="J70" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="K70" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="L70" s="8"/>
+      <c r="M70" s="20"/>
+      <c r="N70" s="21"/>
+      <c r="O70" s="20"/>
+      <c r="P70" s="25"/>
+      <c r="Q70" s="25"/>
+      <c r="R70" s="25"/>
+      <c r="S70" s="26"/>
+      <c r="T70" s="27"/>
+    </row>
+    <row r="71" spans="1:20" s="28" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A71" s="8">
         <v>70</v>
       </c>
-      <c r="B71" s="30" t="s">
-        <v>217</v>
-      </c>
-      <c r="C71" s="31" t="s">
-        <v>211</v>
-      </c>
-      <c r="D71" s="31" t="s">
-        <v>218</v>
-      </c>
-      <c r="E71" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="F71" s="32">
-        <v>42475</v>
-      </c>
-      <c r="G71" s="32" t="s">
-        <v>213</v>
-      </c>
-      <c r="H71" s="32">
-        <v>42475</v>
-      </c>
-      <c r="I71" s="31"/>
-      <c r="J71" s="33" t="s">
-        <v>219</v>
-      </c>
-      <c r="K71" s="31" t="s">
-        <v>215</v>
-      </c>
-      <c r="L71" s="31"/>
-      <c r="M71" s="33"/>
-      <c r="N71" s="32"/>
-      <c r="O71" s="33"/>
-      <c r="P71" s="34"/>
-      <c r="Q71" s="34"/>
-      <c r="R71" s="34"/>
-      <c r="S71" s="35"/>
-      <c r="T71" s="36"/>
+      <c r="B71" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F71" s="21">
+        <v>42478</v>
+      </c>
+      <c r="G71" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H71" s="21">
+        <v>42478</v>
+      </c>
+      <c r="I71" s="8"/>
+      <c r="J71" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="K71" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="L71" s="8"/>
+      <c r="M71" s="20"/>
+      <c r="N71" s="21"/>
+      <c r="O71" s="20"/>
+      <c r="P71" s="25"/>
+      <c r="Q71" s="25"/>
+      <c r="R71" s="25"/>
+      <c r="S71" s="26"/>
+      <c r="T71" s="27"/>
     </row>
     <row r="72" spans="1:20" s="37" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A72" s="8">
         <v>71</v>
       </c>
       <c r="B72" s="30" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="C72" s="31" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="D72" s="31" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="E72" s="31" t="s">
         <v>213</v>
@@ -4907,7 +4936,7 @@
       </c>
       <c r="I72" s="31"/>
       <c r="J72" s="33" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="K72" s="31" t="s">
         <v>215</v>
@@ -4918,7 +4947,9 @@
       <c r="O72" s="33"/>
       <c r="P72" s="34"/>
       <c r="Q72" s="34"/>
-      <c r="R72" s="34"/>
+      <c r="R72" s="34" t="s">
+        <v>216</v>
+      </c>
       <c r="S72" s="35"/>
       <c r="T72" s="36"/>
     </row>
@@ -4927,13 +4958,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="30" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C73" s="31" t="s">
         <v>211</v>
       </c>
       <c r="D73" s="31" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="E73" s="31" t="s">
         <v>213</v>
@@ -4949,7 +4980,7 @@
       </c>
       <c r="I73" s="31"/>
       <c r="J73" s="33" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="K73" s="31" t="s">
         <v>215</v>
@@ -4969,13 +5000,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C74" s="31" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="D74" s="31" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="E74" s="31" t="s">
         <v>213</v>
@@ -4991,7 +5022,7 @@
       </c>
       <c r="I74" s="31"/>
       <c r="J74" s="33" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="K74" s="31" t="s">
         <v>215</v>
@@ -5011,13 +5042,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="30" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C75" s="31" t="s">
         <v>211</v>
       </c>
       <c r="D75" s="31" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="E75" s="31" t="s">
         <v>213</v>
@@ -5053,13 +5084,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="30" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C76" s="31" t="s">
         <v>211</v>
       </c>
       <c r="D76" s="31" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="E76" s="31" t="s">
         <v>213</v>
@@ -5090,111 +5121,105 @@
       <c r="S76" s="35"/>
       <c r="T76" s="36"/>
     </row>
-    <row r="77" spans="1:20" s="28" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:20" s="37" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A77" s="8">
         <v>76</v>
       </c>
-      <c r="B77" s="23" t="s">
-        <v>231</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D77" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="E77" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F77" s="21">
-        <v>42478</v>
-      </c>
-      <c r="G77" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="H77" s="21">
-        <v>42478</v>
-      </c>
-      <c r="I77" s="8"/>
-      <c r="J77" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="K77" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="L77" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="M77" s="20"/>
-      <c r="N77" s="21"/>
-      <c r="O77" s="20"/>
-      <c r="P77" s="25"/>
-      <c r="Q77" s="25"/>
-      <c r="R77" s="38"/>
-      <c r="S77" s="26" t="s">
-        <v>237</v>
-      </c>
-      <c r="T77" s="27"/>
-    </row>
-    <row r="78" spans="1:20" s="28" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B77" s="30" t="s">
+        <v>228</v>
+      </c>
+      <c r="C77" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="D77" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="E77" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="F77" s="32">
+        <v>42475</v>
+      </c>
+      <c r="G77" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="H77" s="32">
+        <v>42475</v>
+      </c>
+      <c r="I77" s="31"/>
+      <c r="J77" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="K77" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="L77" s="31"/>
+      <c r="M77" s="33"/>
+      <c r="N77" s="32"/>
+      <c r="O77" s="33"/>
+      <c r="P77" s="34"/>
+      <c r="Q77" s="34"/>
+      <c r="R77" s="34"/>
+      <c r="S77" s="35"/>
+      <c r="T77" s="36"/>
+    </row>
+    <row r="78" spans="1:20" s="37" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A78" s="8">
         <v>77</v>
       </c>
-      <c r="B78" s="23" t="s">
-        <v>238</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="E78" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F78" s="21">
-        <v>42478</v>
-      </c>
-      <c r="G78" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="H78" s="21">
-        <v>42478</v>
-      </c>
-      <c r="I78" s="8"/>
-      <c r="J78" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="K78" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="L78" s="20"/>
-      <c r="M78" s="20"/>
-      <c r="N78" s="21"/>
-      <c r="O78" s="20"/>
-      <c r="P78" s="25"/>
-      <c r="Q78" s="25"/>
-      <c r="R78" s="38"/>
-      <c r="S78" s="26" t="s">
-        <v>242</v>
-      </c>
-      <c r="T78" s="27"/>
-    </row>
-    <row r="79" spans="1:20" s="28" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="B78" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="C78" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="D78" s="31" t="s">
+        <v>230</v>
+      </c>
+      <c r="E78" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="F78" s="32">
+        <v>42475</v>
+      </c>
+      <c r="G78" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="H78" s="32">
+        <v>42475</v>
+      </c>
+      <c r="I78" s="31"/>
+      <c r="J78" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="K78" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="L78" s="31"/>
+      <c r="M78" s="33"/>
+      <c r="N78" s="32"/>
+      <c r="O78" s="33"/>
+      <c r="P78" s="34"/>
+      <c r="Q78" s="34"/>
+      <c r="R78" s="34"/>
+      <c r="S78" s="35"/>
+      <c r="T78" s="36"/>
+    </row>
+    <row r="79" spans="1:20" s="28" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="8">
         <v>78</v>
       </c>
       <c r="B79" s="23" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>196</v>
+        <v>28</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>186</v>
+        <v>32</v>
       </c>
       <c r="F79" s="21">
         <v>42478</v>
@@ -5207,12 +5232,14 @@
       </c>
       <c r="I79" s="8"/>
       <c r="J79" s="8" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="K79" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="L79" s="20"/>
+        <v>235</v>
+      </c>
+      <c r="L79" s="8" t="s">
+        <v>236</v>
+      </c>
       <c r="M79" s="20"/>
       <c r="N79" s="21"/>
       <c r="O79" s="20"/>
@@ -5220,25 +5247,25 @@
       <c r="Q79" s="25"/>
       <c r="R79" s="38"/>
       <c r="S79" s="26" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="T79" s="27"/>
     </row>
-    <row r="80" spans="1:20" s="28" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:20" s="28" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="8">
         <v>79</v>
       </c>
       <c r="B80" s="23" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>139</v>
+        <v>196</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>239</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>130</v>
+        <v>32</v>
       </c>
       <c r="F80" s="21">
         <v>42478</v>
@@ -5251,12 +5278,12 @@
       </c>
       <c r="I80" s="8"/>
       <c r="J80" s="8" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="K80" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="L80" s="8"/>
+        <v>241</v>
+      </c>
+      <c r="L80" s="20"/>
       <c r="M80" s="20"/>
       <c r="N80" s="21"/>
       <c r="O80" s="20"/>
@@ -5273,34 +5300,34 @@
         <v>80</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>139</v>
+        <v>196</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>130</v>
+        <v>186</v>
       </c>
       <c r="F81" s="21">
         <v>42478</v>
       </c>
       <c r="G81" s="21" t="s">
-        <v>130</v>
+        <v>32</v>
       </c>
       <c r="H81" s="21">
         <v>42478</v>
       </c>
       <c r="I81" s="8"/>
       <c r="J81" s="8" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="K81" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="L81" s="8"/>
+      <c r="L81" s="20"/>
       <c r="M81" s="20"/>
       <c r="N81" s="21"/>
       <c r="O81" s="20"/>
@@ -5308,7 +5335,7 @@
       <c r="Q81" s="25"/>
       <c r="R81" s="38"/>
       <c r="S81" s="26" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="T81" s="27"/>
     </row>
@@ -5317,13 +5344,13 @@
         <v>81</v>
       </c>
       <c r="B82" s="23" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>28</v>
+        <v>139</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>130</v>
@@ -5339,14 +5366,12 @@
       </c>
       <c r="I82" s="8"/>
       <c r="J82" s="8" t="s">
-        <v>255</v>
+        <v>233</v>
       </c>
       <c r="K82" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="L82" s="8" t="s">
-        <v>256</v>
-      </c>
+      <c r="L82" s="8"/>
       <c r="M82" s="20"/>
       <c r="N82" s="21"/>
       <c r="O82" s="20"/>
@@ -5354,7 +5379,7 @@
       <c r="Q82" s="25"/>
       <c r="R82" s="38"/>
       <c r="S82" s="26" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="T82" s="27"/>
     </row>
@@ -5363,13 +5388,13 @@
         <v>82</v>
       </c>
       <c r="B83" s="23" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C83" s="8" t="s">
         <v>139</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>147</v>
+        <v>250</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>130</v>
@@ -5385,22 +5410,20 @@
       </c>
       <c r="I83" s="8"/>
       <c r="J83" s="8" t="s">
-        <v>259</v>
+        <v>240</v>
       </c>
       <c r="K83" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="L83" s="8" t="s">
-        <v>260</v>
-      </c>
+      <c r="L83" s="8"/>
       <c r="M83" s="20"/>
       <c r="N83" s="21"/>
       <c r="O83" s="20"/>
       <c r="P83" s="25"/>
       <c r="Q83" s="25"/>
-      <c r="R83" s="39"/>
+      <c r="R83" s="38"/>
       <c r="S83" s="26" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="T83" s="27"/>
     </row>
@@ -5409,42 +5432,44 @@
         <v>83</v>
       </c>
       <c r="B84" s="23" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>139</v>
+        <v>28</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>186</v>
+        <v>130</v>
       </c>
       <c r="F84" s="21">
         <v>42478</v>
       </c>
       <c r="G84" s="21" t="s">
-        <v>186</v>
+        <v>130</v>
       </c>
       <c r="H84" s="21">
         <v>42478</v>
       </c>
       <c r="I84" s="8"/>
       <c r="J84" s="8" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="K84" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="L84" s="8"/>
+      <c r="L84" s="8" t="s">
+        <v>256</v>
+      </c>
       <c r="M84" s="20"/>
       <c r="N84" s="21"/>
       <c r="O84" s="20"/>
       <c r="P84" s="25"/>
       <c r="Q84" s="25"/>
-      <c r="R84" s="39"/>
+      <c r="R84" s="38"/>
       <c r="S84" s="26" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="T84" s="27"/>
     </row>
@@ -5453,13 +5478,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="23" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>139</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>244</v>
+        <v>147</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>130</v>
@@ -5475,12 +5500,14 @@
       </c>
       <c r="I85" s="8"/>
       <c r="J85" s="8" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="K85" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="L85" s="8"/>
+      <c r="L85" s="8" t="s">
+        <v>260</v>
+      </c>
       <c r="M85" s="20"/>
       <c r="N85" s="21"/>
       <c r="O85" s="20"/>
@@ -5488,7 +5515,7 @@
       <c r="Q85" s="25"/>
       <c r="R85" s="39"/>
       <c r="S85" s="26" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="T85" s="27"/>
     </row>
@@ -5497,16 +5524,16 @@
         <v>85</v>
       </c>
       <c r="B86" s="23" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>28</v>
+        <v>139</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>130</v>
+        <v>186</v>
       </c>
       <c r="F86" s="21">
         <v>42478</v>
@@ -5522,19 +5549,17 @@
         <v>263</v>
       </c>
       <c r="K86" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="L86" s="8" t="s">
-        <v>269</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="L86" s="8"/>
       <c r="M86" s="20"/>
       <c r="N86" s="21"/>
       <c r="O86" s="20"/>
-      <c r="P86" s="17"/>
-      <c r="Q86" s="17"/>
+      <c r="P86" s="25"/>
+      <c r="Q86" s="25"/>
       <c r="R86" s="39"/>
       <c r="S86" s="26" t="s">
-        <v>237</v>
+        <v>264</v>
       </c>
       <c r="T86" s="27"/>
     </row>
@@ -5543,7 +5568,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="23" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>139</v>
@@ -5558,7 +5583,7 @@
         <v>42478</v>
       </c>
       <c r="G87" s="21" t="s">
-        <v>186</v>
+        <v>130</v>
       </c>
       <c r="H87" s="21">
         <v>42478</v>
@@ -5574,8 +5599,8 @@
       <c r="M87" s="20"/>
       <c r="N87" s="21"/>
       <c r="O87" s="20"/>
-      <c r="P87" s="17"/>
-      <c r="Q87" s="17"/>
+      <c r="P87" s="25"/>
+      <c r="Q87" s="25"/>
       <c r="R87" s="39"/>
       <c r="S87" s="26" t="s">
         <v>247</v>
@@ -5587,13 +5612,13 @@
         <v>87</v>
       </c>
       <c r="B88" s="23" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>139</v>
+        <v>28</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>130</v>
@@ -5602,20 +5627,20 @@
         <v>42478</v>
       </c>
       <c r="G88" s="21" t="s">
-        <v>130</v>
+        <v>186</v>
       </c>
       <c r="H88" s="21">
         <v>42478</v>
       </c>
       <c r="I88" s="8"/>
       <c r="J88" s="8" t="s">
-        <v>240</v>
+        <v>263</v>
       </c>
       <c r="K88" s="8" t="s">
         <v>235</v>
       </c>
       <c r="L88" s="8" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="M88" s="20"/>
       <c r="N88" s="21"/>
@@ -5624,7 +5649,7 @@
       <c r="Q88" s="17"/>
       <c r="R88" s="39"/>
       <c r="S88" s="26" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="T88" s="27"/>
     </row>
@@ -5633,13 +5658,13 @@
         <v>88</v>
       </c>
       <c r="B89" s="23" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C89" s="8" t="s">
         <v>139</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>130</v>
@@ -5648,21 +5673,19 @@
         <v>42478</v>
       </c>
       <c r="G89" s="21" t="s">
-        <v>32</v>
+        <v>186</v>
       </c>
       <c r="H89" s="21">
         <v>42478</v>
       </c>
       <c r="I89" s="8"/>
       <c r="J89" s="8" t="s">
-        <v>255</v>
+        <v>266</v>
       </c>
       <c r="K89" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="L89" s="8" t="s">
-        <v>272</v>
-      </c>
+      <c r="L89" s="8"/>
       <c r="M89" s="20"/>
       <c r="N89" s="21"/>
       <c r="O89" s="20"/>
@@ -5670,7 +5693,7 @@
       <c r="Q89" s="17"/>
       <c r="R89" s="39"/>
       <c r="S89" s="26" t="s">
-        <v>274</v>
+        <v>247</v>
       </c>
       <c r="T89" s="27"/>
     </row>
@@ -5679,10 +5702,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="23" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>196</v>
+        <v>139</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>254</v>
@@ -5701,7 +5724,7 @@
       </c>
       <c r="I90" s="8"/>
       <c r="J90" s="8" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="K90" s="8" t="s">
         <v>235</v>
@@ -5716,7 +5739,7 @@
       <c r="Q90" s="17"/>
       <c r="R90" s="39"/>
       <c r="S90" s="26" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="T90" s="27"/>
     </row>
@@ -5725,13 +5748,13 @@
         <v>90</v>
       </c>
       <c r="B91" s="23" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>196</v>
+        <v>139</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>130</v>
@@ -5740,19 +5763,21 @@
         <v>42478</v>
       </c>
       <c r="G91" s="21" t="s">
-        <v>130</v>
+        <v>32</v>
       </c>
       <c r="H91" s="21">
         <v>42478</v>
       </c>
       <c r="I91" s="8"/>
       <c r="J91" s="8" t="s">
-        <v>233</v>
+        <v>255</v>
       </c>
       <c r="K91" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="L91" s="8"/>
+      <c r="L91" s="8" t="s">
+        <v>272</v>
+      </c>
       <c r="M91" s="20"/>
       <c r="N91" s="21"/>
       <c r="O91" s="20"/>
@@ -5760,7 +5785,7 @@
       <c r="Q91" s="17"/>
       <c r="R91" s="39"/>
       <c r="S91" s="26" t="s">
-        <v>242</v>
+        <v>274</v>
       </c>
       <c r="T91" s="27"/>
     </row>
@@ -5769,13 +5794,13 @@
         <v>91</v>
       </c>
       <c r="B92" s="23" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C92" s="8" t="s">
         <v>196</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>130</v>
@@ -5794,7 +5819,7 @@
         <v>255</v>
       </c>
       <c r="K92" s="8" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="L92" s="8" t="s">
         <v>272</v>
@@ -5815,13 +5840,13 @@
         <v>92</v>
       </c>
       <c r="B93" s="23" t="s">
-        <v>91</v>
+        <v>276</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>139</v>
+        <v>196</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>130</v>
@@ -5837,14 +5862,12 @@
       </c>
       <c r="I93" s="8"/>
       <c r="J93" s="8" t="s">
-        <v>255</v>
+        <v>233</v>
       </c>
       <c r="K93" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="L93" s="8" t="s">
-        <v>272</v>
-      </c>
+      <c r="L93" s="8"/>
       <c r="M93" s="20"/>
       <c r="N93" s="21"/>
       <c r="O93" s="20"/>
@@ -5852,45 +5875,101 @@
       <c r="Q93" s="17"/>
       <c r="R93" s="39"/>
       <c r="S93" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="T93" s="27"/>
+    </row>
+    <row r="94" spans="1:20" s="28" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A94" s="8">
+        <v>93</v>
+      </c>
+      <c r="B94" s="23" t="s">
+        <v>277</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="E94" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="F94" s="21">
+        <v>42478</v>
+      </c>
+      <c r="G94" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="H94" s="21">
+        <v>42478</v>
+      </c>
+      <c r="I94" s="8"/>
+      <c r="J94" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="K94" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="L94" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="M94" s="20"/>
+      <c r="N94" s="21"/>
+      <c r="O94" s="20"/>
+      <c r="P94" s="17"/>
+      <c r="Q94" s="17"/>
+      <c r="R94" s="39"/>
+      <c r="S94" s="26" t="s">
         <v>274</v>
       </c>
-      <c r="T93" s="27"/>
-    </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A94" s="7"/>
-      <c r="B94" s="4"/>
-      <c r="C94" s="7"/>
-      <c r="D94" s="7"/>
-      <c r="E94" s="7"/>
-      <c r="F94" s="5"/>
-      <c r="G94" s="7"/>
-      <c r="H94" s="5"/>
-      <c r="I94" s="6"/>
-      <c r="J94" s="7"/>
-      <c r="K94" s="7"/>
-      <c r="L94" s="7"/>
-      <c r="M94" s="7"/>
-      <c r="N94" s="5"/>
-      <c r="O94" s="4"/>
-      <c r="S94" s="4"/>
-    </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A95" s="7"/>
-      <c r="B95" s="4"/>
-      <c r="C95" s="7"/>
-      <c r="D95" s="7"/>
-      <c r="E95" s="7"/>
-      <c r="F95" s="5"/>
-      <c r="G95" s="7"/>
-      <c r="H95" s="5"/>
-      <c r="I95" s="6"/>
-      <c r="J95" s="7"/>
-      <c r="K95" s="7"/>
-      <c r="L95" s="7"/>
-      <c r="M95" s="7"/>
-      <c r="N95" s="5"/>
-      <c r="O95" s="4"/>
-      <c r="S95" s="4"/>
+      <c r="T94" s="27"/>
+    </row>
+    <row r="95" spans="1:20" s="28" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A95" s="8">
+        <v>94</v>
+      </c>
+      <c r="B95" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="E95" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="F95" s="21">
+        <v>42478</v>
+      </c>
+      <c r="G95" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="H95" s="21">
+        <v>42478</v>
+      </c>
+      <c r="I95" s="8"/>
+      <c r="J95" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="K95" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="L95" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="M95" s="20"/>
+      <c r="N95" s="21"/>
+      <c r="O95" s="20"/>
+      <c r="P95" s="17"/>
+      <c r="Q95" s="17"/>
+      <c r="R95" s="39"/>
+      <c r="S95" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="T95" s="27"/>
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A96" s="7"/>
@@ -5945,6 +6024,42 @@
       <c r="N98" s="5"/>
       <c r="O98" s="4"/>
       <c r="S98" s="4"/>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A99" s="7"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="7"/>
+      <c r="D99" s="7"/>
+      <c r="E99" s="7"/>
+      <c r="F99" s="5"/>
+      <c r="G99" s="7"/>
+      <c r="H99" s="5"/>
+      <c r="I99" s="6"/>
+      <c r="J99" s="7"/>
+      <c r="K99" s="7"/>
+      <c r="L99" s="7"/>
+      <c r="M99" s="7"/>
+      <c r="N99" s="5"/>
+      <c r="O99" s="4"/>
+      <c r="S99" s="4"/>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A100" s="7"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="7"/>
+      <c r="E100" s="7"/>
+      <c r="F100" s="5"/>
+      <c r="G100" s="7"/>
+      <c r="H100" s="5"/>
+      <c r="I100" s="6"/>
+      <c r="J100" s="7"/>
+      <c r="K100" s="7"/>
+      <c r="L100" s="7"/>
+      <c r="M100" s="7"/>
+      <c r="N100" s="5"/>
+      <c r="O100" s="4"/>
+      <c r="S100" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>